<commit_message>
Updated Banner; added statics
</commit_message>
<xml_diff>
--- a/data/word_data.xlsx
+++ b/data/word_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\anp-website\alexandpedro.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9692A454-22A5-4DAF-8A68-06FB6F0F9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F480EBF0-295F-46A4-8419-10E24F99DDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="word_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="5477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7161" uniqueCount="5497">
   <si>
     <t>english</t>
   </si>
@@ -16505,6 +16505,66 @@
   </si>
   <si>
     <t>酵母</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>magnetic flux</t>
+  </si>
+  <si>
+    <t>磁束</t>
+  </si>
+  <si>
+    <t>密度</t>
+  </si>
+  <si>
+    <t>mitudo</t>
+  </si>
+  <si>
+    <t>magutaba</t>
+  </si>
+  <si>
+    <t>luminous flux</t>
+  </si>
+  <si>
+    <t>光束</t>
+  </si>
+  <si>
+    <t>zûtaba</t>
+  </si>
+  <si>
+    <t>zu^taba</t>
+  </si>
+  <si>
+    <t>磁化</t>
+  </si>
+  <si>
+    <t>magnetization</t>
+  </si>
+  <si>
+    <t>共栄</t>
+  </si>
+  <si>
+    <t>co-prosperity</t>
+  </si>
+  <si>
+    <t>maguchen</t>
+  </si>
+  <si>
+    <t>tanawi</t>
+  </si>
+  <si>
+    <t>magucen</t>
+  </si>
+  <si>
+    <t>tannaku</t>
+  </si>
+  <si>
+    <t>hara</t>
+  </si>
+  <si>
+    <t>xitukak</t>
   </si>
 </sst>
 </file>
@@ -17565,11 +17625,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3139"/>
+  <dimension ref="A1:L3144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3070" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3078" sqref="H3078"/>
+      <pane ySplit="1" topLeftCell="A661" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B738" sqref="B738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26261,6 +26321,9 @@
       <c r="B797" s="1" t="s">
         <v>685</v>
       </c>
+      <c r="C797" s="1" t="s">
+        <v>5496</v>
+      </c>
       <c r="E797" s="1" t="s">
         <v>64</v>
       </c>
@@ -47243,6 +47306,12 @@
       <c r="A3042" s="8" t="s">
         <v>4099</v>
       </c>
+      <c r="B3042" s="1" t="s">
+        <v>5495</v>
+      </c>
+      <c r="H3042" s="1" t="s">
+        <v>4690</v>
+      </c>
     </row>
     <row r="3043" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3043" s="8" t="s">
@@ -47429,6 +47498,9 @@
       <c r="F3057" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H3057" s="1" t="s">
+        <v>4690</v>
+      </c>
     </row>
     <row r="3058" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3058" s="15" t="s">
@@ -48468,6 +48540,12 @@
       <c r="A3119" s="1" t="s">
         <v>5344</v>
       </c>
+      <c r="B3119" s="1" t="s">
+        <v>5494</v>
+      </c>
+      <c r="C3119" s="1" t="s">
+        <v>5494</v>
+      </c>
       <c r="E3119" s="1" t="s">
         <v>10</v>
       </c>
@@ -48879,6 +48957,106 @@
       </c>
       <c r="H3139" s="1" t="s">
         <v>5472</v>
+      </c>
+    </row>
+    <row r="3140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3140" s="1" t="s">
+        <v>5477</v>
+      </c>
+      <c r="B3140" s="1" t="s">
+        <v>5481</v>
+      </c>
+      <c r="C3140" s="1" t="s">
+        <v>5481</v>
+      </c>
+      <c r="E3140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3140" s="1" t="s">
+        <v>5480</v>
+      </c>
+    </row>
+    <row r="3141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3141" s="1" t="s">
+        <v>5478</v>
+      </c>
+      <c r="B3141" s="1" t="s">
+        <v>5482</v>
+      </c>
+      <c r="C3141" s="1" t="s">
+        <v>5482</v>
+      </c>
+      <c r="E3141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3141" s="1" t="s">
+        <v>5479</v>
+      </c>
+    </row>
+    <row r="3142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3142" s="1" t="s">
+        <v>5483</v>
+      </c>
+      <c r="B3142" s="1" t="s">
+        <v>5485</v>
+      </c>
+      <c r="C3142" s="1" t="s">
+        <v>5486</v>
+      </c>
+      <c r="E3142" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3142" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3142" s="1" t="s">
+        <v>5484</v>
+      </c>
+    </row>
+    <row r="3143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3143" s="1" t="s">
+        <v>5488</v>
+      </c>
+      <c r="B3143" s="1" t="s">
+        <v>5491</v>
+      </c>
+      <c r="C3143" s="1" t="s">
+        <v>5493</v>
+      </c>
+      <c r="E3143" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3143" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3143" s="1" t="s">
+        <v>5487</v>
+      </c>
+    </row>
+    <row r="3144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3144" s="1" t="s">
+        <v>5490</v>
+      </c>
+      <c r="B3144" s="1" t="s">
+        <v>5492</v>
+      </c>
+      <c r="C3144" s="1" t="s">
+        <v>5492</v>
+      </c>
+      <c r="E3144" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3144" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3144" s="1" t="s">
+        <v>5489</v>
       </c>
     </row>
   </sheetData>
@@ -48886,7 +49064,7 @@
     <sortCondition ref="A2:A3098"/>
   </sortState>
   <phoneticPr fontId="26" type="noConversion"/>
-  <conditionalFormatting sqref="B5110:B1048576 B2039:B2085 B356:B2025 B2087:B2097 B2099:B2105 B1:B354">
+  <conditionalFormatting sqref="B5110:B1048576 B2039:B2085 B356:B2025 B2087:B2097 B2099:B2105 B1:B354 C797">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B355">
@@ -48915,7 +49093,7 @@
   <conditionalFormatting sqref="A3097:A1048576 A2106:A3095 A1:A2104">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3105 B1:B1048576">
+  <conditionalFormatting sqref="C3105 B1:B1048576 C797">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3097:A1048576 A3077:A3095 A2039:A2104 A1:A2025">

</xml_diff>